<commit_message>
- Modify web layout - Refactor desktop app code
</commit_message>
<xml_diff>
--- a/docs/mocks/MOCK_DATA.xlsx
+++ b/docs/mocks/MOCK_DATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lex\Documents\Schoolwork\S2-CB04\Projects\s2-synthesis-duelsys\docs\mocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BF7A4F-B1D3-4E5E-976E-4A435645AC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E378B6-9302-4E70-97F3-AE5ED58D763F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2835" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2265" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="89">
   <si>
     <t>first_name</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>DB ID's</t>
   </si>
 </sst>
 </file>
@@ -640,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -653,7 +656,7 @@
     <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -669,8 +672,11 @@
       <c r="E1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -686,8 +692,11 @@
       <c r="E2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -703,8 +712,11 @@
       <c r="E3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -720,8 +732,11 @@
       <c r="E4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -737,8 +752,11 @@
       <c r="E5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -754,8 +772,11 @@
       <c r="E6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -771,8 +792,11 @@
       <c r="E7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -788,8 +812,11 @@
       <c r="E8" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -805,8 +832,11 @@
       <c r="E9" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -822,8 +852,11 @@
       <c r="E10" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -839,8 +872,11 @@
       <c r="E11" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -856,8 +892,11 @@
       <c r="E12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -873,8 +912,11 @@
       <c r="E13" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -890,8 +932,11 @@
       <c r="E14" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -907,8 +952,11 @@
       <c r="E15" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -924,8 +972,11 @@
       <c r="E16" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -941,8 +992,11 @@
       <c r="E17" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -958,8 +1012,11 @@
       <c r="E18" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -975,8 +1032,11 @@
       <c r="E19" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -992,8 +1052,11 @@
       <c r="E20" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1008,6 +1071,9 @@
       </c>
       <c r="E21" t="s">
         <v>85</v>
+      </c>
+      <c r="F21">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>